<commit_message>
Fixed NBA binary for all sheets, some missing though, added combine metrics
</commit_message>
<xml_diff>
--- a/NCAA/master_teams.xlsx
+++ b/NCAA/master_teams.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\PycharmProjects\MQP_Stat\NCAA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{16C60213-5C14-41C8-9CB7-63145B66AAFF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="18" windowWidth="16098" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="739">
   <si>
     <t>ID</t>
   </si>
@@ -1114,16 +1120,16 @@
     <t>American</t>
   </si>
   <si>
-    <t xml:space="preserve">Appalachian State </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arizona </t>
+    <t>Appalachian State </t>
+  </si>
+  <si>
+    <t>Arizona </t>
   </si>
   <si>
     <t>Arizona State</t>
   </si>
   <si>
-    <t xml:space="preserve">Arkansas </t>
+    <t>Arkansas </t>
   </si>
   <si>
     <t>Little Rock</t>
@@ -1138,13 +1144,13 @@
     <t>Army</t>
   </si>
   <si>
-    <t xml:space="preserve">Auburn </t>
+    <t>Auburn </t>
   </si>
   <si>
     <t>Austin Peay</t>
   </si>
   <si>
-    <t xml:space="preserve">Ball State </t>
+    <t>Ball State </t>
   </si>
   <si>
     <t>Baylor</t>
@@ -1192,7 +1198,7 @@
     <t>Buffalo</t>
   </si>
   <si>
-    <t xml:space="preserve">Butler </t>
+    <t>Butler </t>
   </si>
   <si>
     <t>Cal Poly</t>
@@ -1234,7 +1240,7 @@
     <t>Central Arkansas</t>
   </si>
   <si>
-    <t xml:space="preserve">Central Connecticut State </t>
+    <t>Central Connecticut State </t>
   </si>
   <si>
     <t>Central Florida</t>
@@ -1255,7 +1261,7 @@
     <t>Chicago State</t>
   </si>
   <si>
-    <t xml:space="preserve">Cincinnati </t>
+    <t>Cincinnati </t>
   </si>
   <si>
     <t>Citadel</t>
@@ -1285,7 +1291,7 @@
     <t>Columbia</t>
   </si>
   <si>
-    <t xml:space="preserve">Connecticut </t>
+    <t>Connecticut </t>
   </si>
   <si>
     <t>Coppin State</t>
@@ -1294,7 +1300,7 @@
     <t>Cornell</t>
   </si>
   <si>
-    <t xml:space="preserve">Creighton </t>
+    <t>Creighton </t>
   </si>
   <si>
     <t>Dartmouth</t>
@@ -1303,7 +1309,7 @@
     <t>Davidson</t>
   </si>
   <si>
-    <t xml:space="preserve">Dayton </t>
+    <t>Dayton </t>
   </si>
   <si>
     <t>Delaware</t>
@@ -1315,7 +1321,7 @@
     <t>Denver</t>
   </si>
   <si>
-    <t xml:space="preserve">DePaul </t>
+    <t>DePaul </t>
   </si>
   <si>
     <t>Detroit Mercy</t>
@@ -1327,7 +1333,7 @@
     <t>Drexel</t>
   </si>
   <si>
-    <t xml:space="preserve">Duke </t>
+    <t>Duke </t>
   </si>
   <si>
     <t>Duquesne</t>
@@ -1363,7 +1369,7 @@
     <t>Fairleigh Dickinson</t>
   </si>
   <si>
-    <t xml:space="preserve">Florida </t>
+    <t>Florida </t>
   </si>
   <si>
     <t>Florida A&amp;M</t>
@@ -1384,7 +1390,7 @@
     <t>Fordham</t>
   </si>
   <si>
-    <t xml:space="preserve">Fresno State </t>
+    <t>Fresno State </t>
   </si>
   <si>
     <t>Furman</t>
@@ -1414,7 +1420,7 @@
     <t>Georgia Tech</t>
   </si>
   <si>
-    <t xml:space="preserve">Gonzaga </t>
+    <t>Gonzaga </t>
   </si>
   <si>
     <t>Grambling</t>
@@ -1441,7 +1447,7 @@
     <t>High Point</t>
   </si>
   <si>
-    <t xml:space="preserve">Hofstra </t>
+    <t>Hofstra </t>
   </si>
   <si>
     <t>Holy Cross</t>
@@ -1462,7 +1468,7 @@
     <t>Idaho State</t>
   </si>
   <si>
-    <t xml:space="preserve">Illinois </t>
+    <t>Illinois </t>
   </si>
   <si>
     <t>Illinois-Chicago</t>
@@ -1474,19 +1480,19 @@
     <t>Incarnate Word</t>
   </si>
   <si>
-    <t xml:space="preserve">Indiana </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indiana State </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iona </t>
+    <t>Indiana </t>
+  </si>
+  <si>
+    <t>Indiana State </t>
+  </si>
+  <si>
+    <t>Iona </t>
   </si>
   <si>
     <t>Iowa</t>
   </si>
   <si>
-    <t xml:space="preserve">Iowa State </t>
+    <t>Iowa State </t>
   </si>
   <si>
     <t>Fort Wayne</t>
@@ -1495,7 +1501,7 @@
     <t>IUPUI</t>
   </si>
   <si>
-    <t xml:space="preserve">Jackson State </t>
+    <t>Jackson State </t>
   </si>
   <si>
     <t>Jacksonville</t>
@@ -1507,7 +1513,7 @@
     <t>James Madison</t>
   </si>
   <si>
-    <t xml:space="preserve">Kansas </t>
+    <t>Kansas </t>
   </si>
   <si>
     <t>Kansas State</t>
@@ -1519,16 +1525,16 @@
     <t>Kent State</t>
   </si>
   <si>
-    <t xml:space="preserve">Kentucky </t>
+    <t>Kentucky </t>
   </si>
   <si>
     <t>La Salle</t>
   </si>
   <si>
-    <t xml:space="preserve">Lafayette </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lamar </t>
+    <t>Lafayette </t>
+  </si>
+  <si>
+    <t>Lamar </t>
   </si>
   <si>
     <t>Lehigh</t>
@@ -1549,19 +1555,19 @@
     <t>Longwood</t>
   </si>
   <si>
-    <t xml:space="preserve">Louisiana </t>
+    <t>Louisiana </t>
   </si>
   <si>
     <t>Louisiana-Monroe</t>
   </si>
   <si>
-    <t xml:space="preserve">Louisiana State </t>
+    <t>Louisiana State </t>
   </si>
   <si>
     <t>Louisiana Tech</t>
   </si>
   <si>
-    <t xml:space="preserve">Louisville </t>
+    <t>Louisville </t>
   </si>
   <si>
     <t>Loyola (IL)</t>
@@ -1588,7 +1594,7 @@
     <t>Marshall</t>
   </si>
   <si>
-    <t xml:space="preserve">Maryland </t>
+    <t>Maryland </t>
   </si>
   <si>
     <t>Maryland-Baltimore County</t>
@@ -1612,7 +1618,7 @@
     <t>Mercer</t>
   </si>
   <si>
-    <t xml:space="preserve">Miami (FL) </t>
+    <t>Miami (FL) </t>
   </si>
   <si>
     <t>Miami (OH)</t>
@@ -1621,7 +1627,7 @@
     <t>Michigan</t>
   </si>
   <si>
-    <t xml:space="preserve">Michigan State </t>
+    <t>Michigan State </t>
   </si>
   <si>
     <t>Middle Tennessee</t>
@@ -1642,7 +1648,7 @@
     <t>Mississippi Valley State</t>
   </si>
   <si>
-    <t xml:space="preserve">Missouri </t>
+    <t>Missouri </t>
   </si>
   <si>
     <t>Missouri-Kansas City</t>
@@ -1687,7 +1693,7 @@
     <t>Nevada</t>
   </si>
   <si>
-    <t xml:space="preserve">Nevada-Las Vegas </t>
+    <t>Nevada-Las Vegas </t>
   </si>
   <si>
     <t>New Hampshire</t>
@@ -1714,7 +1720,7 @@
     <t>Norfolk State</t>
   </si>
   <si>
-    <t xml:space="preserve">North Carolina </t>
+    <t>North Carolina </t>
   </si>
   <si>
     <t>North Carolina-Asheville</t>
@@ -1732,13 +1738,13 @@
     <t>North Carolina State</t>
   </si>
   <si>
-    <t xml:space="preserve">North Carolina-Wilmington </t>
+    <t>North Carolina-Wilmington </t>
   </si>
   <si>
     <t>North Dakota</t>
   </si>
   <si>
-    <t xml:space="preserve">North Dakota State </t>
+    <t>North Dakota State </t>
   </si>
   <si>
     <t>North Florida</t>
@@ -1750,7 +1756,7 @@
     <t>Northeastern</t>
   </si>
   <si>
-    <t xml:space="preserve">Northern Arizona </t>
+    <t>Northern Arizona </t>
   </si>
   <si>
     <t>Northern Colorado</t>
@@ -1780,13 +1786,13 @@
     <t>Ohio</t>
   </si>
   <si>
-    <t xml:space="preserve">Ohio State </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oklahoma </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oklahoma State </t>
+    <t>Ohio State </t>
+  </si>
+  <si>
+    <t>Oklahoma </t>
+  </si>
+  <si>
+    <t>Oklahoma State </t>
   </si>
   <si>
     <t>Old Dominion</t>
@@ -1795,7 +1801,7 @@
     <t>Oral Roberts</t>
   </si>
   <si>
-    <t xml:space="preserve">Oregon </t>
+    <t>Oregon </t>
   </si>
   <si>
     <t>Oregon State</t>
@@ -1807,10 +1813,10 @@
     <t>Penn State</t>
   </si>
   <si>
-    <t xml:space="preserve">Pennsylvania </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pepperdine </t>
+    <t>Pennsylvania </t>
+  </si>
+  <si>
+    <t>Pepperdine </t>
   </si>
   <si>
     <t>Pittsburgh</t>
@@ -1834,7 +1840,7 @@
     <t>Providence</t>
   </si>
   <si>
-    <t xml:space="preserve">Purdue </t>
+    <t>Purdue </t>
   </si>
   <si>
     <t>Quinnipiac</t>
@@ -1873,7 +1879,7 @@
     <t>Saint Joseph's</t>
   </si>
   <si>
-    <t xml:space="preserve">Saint Louis </t>
+    <t>Saint Louis </t>
   </si>
   <si>
     <t>Saint Mary's (CA)</t>
@@ -1885,7 +1891,7 @@
     <t>Sam Houston State</t>
   </si>
   <si>
-    <t xml:space="preserve">Samford </t>
+    <t>Samford </t>
   </si>
   <si>
     <t>San Diego</t>
@@ -1909,7 +1915,7 @@
     <t>Seattle</t>
   </si>
   <si>
-    <t xml:space="preserve">Seton Hall </t>
+    <t>Seton Hall </t>
   </si>
   <si>
     <t>Siena</t>
@@ -1921,7 +1927,7 @@
     <t>South Carolina</t>
   </si>
   <si>
-    <t xml:space="preserve">South Carolina State </t>
+    <t>South Carolina State </t>
   </si>
   <si>
     <t>South Carolina Upstate</t>
@@ -1936,7 +1942,7 @@
     <t>South Florida</t>
   </si>
   <si>
-    <t xml:space="preserve">Southeast Missouri State </t>
+    <t>Southeast Missouri State </t>
   </si>
   <si>
     <t>Southeastern Louisiana</t>
@@ -1963,16 +1969,16 @@
     <t>Southern Utah</t>
   </si>
   <si>
-    <t xml:space="preserve">St. Bonaventure </t>
+    <t>St. Bonaventure </t>
   </si>
   <si>
     <t>St. Francis (NY)</t>
   </si>
   <si>
-    <t xml:space="preserve">St. John's (NY) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stanford </t>
+    <t>St. John's (NY) </t>
+  </si>
+  <si>
+    <t>Stanford </t>
   </si>
   <si>
     <t>Stephen F. Austin</t>
@@ -1984,13 +1990,13 @@
     <t>Stony Brook</t>
   </si>
   <si>
-    <t xml:space="preserve">Syracuse </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temple </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tennessee </t>
+    <t>Syracuse </t>
+  </si>
+  <si>
+    <t>Temple </t>
+  </si>
+  <si>
+    <t>Tennessee </t>
   </si>
   <si>
     <t>Tennessee-Martin</t>
@@ -2002,7 +2008,7 @@
     <t>Tennessee Tech</t>
   </si>
   <si>
-    <t xml:space="preserve">Texas </t>
+    <t>Texas </t>
   </si>
   <si>
     <t>Texas A&amp;M</t>
@@ -2047,22 +2053,22 @@
     <t>Tulane</t>
   </si>
   <si>
-    <t xml:space="preserve">Tulsa </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UCLA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utah </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utah State </t>
+    <t>Tulsa </t>
+  </si>
+  <si>
+    <t>UCLA </t>
+  </si>
+  <si>
+    <t>Utah </t>
+  </si>
+  <si>
+    <t>Utah State </t>
   </si>
   <si>
     <t>Utah Valley</t>
   </si>
   <si>
-    <t xml:space="preserve">Valparaiso </t>
+    <t>Valparaiso </t>
   </si>
   <si>
     <t>Vanderbilt</t>
@@ -2122,10 +2128,10 @@
     <t>William &amp; Mary</t>
   </si>
   <si>
-    <t xml:space="preserve">Winthrop </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wisconsin </t>
+    <t>Winthrop </t>
+  </si>
+  <si>
+    <t>Wisconsin </t>
   </si>
   <si>
     <t>Wofford</t>
@@ -2144,13 +2150,100 @@
   </si>
   <si>
     <t>Youngstown State</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>alabamaam</t>
+  </si>
+  <si>
+    <t>alabamast</t>
+  </si>
+  <si>
+    <t>albanyst</t>
+  </si>
+  <si>
+    <t>alcornst</t>
+  </si>
+  <si>
+    <t>appalst</t>
+  </si>
+  <si>
+    <t>arizonast</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>uab</t>
+  </si>
+  <si>
+    <t>arkansaslr</t>
+  </si>
+  <si>
+    <t>arkansaspb</t>
+  </si>
+  <si>
+    <t>arkansasst</t>
+  </si>
+  <si>
+    <t>austinpeay</t>
+  </si>
+  <si>
+    <t>ballst</t>
+  </si>
+  <si>
+    <t>bethcook</t>
+  </si>
+  <si>
+    <t>boisest</t>
+  </si>
+  <si>
+    <t>bostoncoll</t>
+  </si>
+  <si>
+    <t>bostonuniv</t>
+  </si>
+  <si>
+    <t>bowlgreen</t>
+  </si>
+  <si>
+    <t>byu</t>
+  </si>
+  <si>
+    <t>buffalost</t>
+  </si>
+  <si>
+    <t>calpoly</t>
+  </si>
+  <si>
+    <t>calstbake</t>
+  </si>
+  <si>
+    <t>calstfull</t>
+  </si>
+  <si>
+    <t>calstnorth</t>
+  </si>
+  <si>
+    <t>ucirvine</t>
+  </si>
+  <si>
+    <t>ucriver</t>
+  </si>
+  <si>
+    <t>ucsb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2213,6 +2306,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2259,7 +2360,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2291,9 +2392,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2325,6 +2444,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2500,22 +2637,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C355"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D355"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="23.5234375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>573</v>
       </c>
@@ -2525,8 +2670,11 @@
       <c r="C2" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -2536,8 +2684,11 @@
       <c r="C3" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -2547,8 +2698,11 @@
       <c r="C4" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -2558,8 +2712,11 @@
       <c r="C5" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -2569,8 +2726,11 @@
       <c r="C6" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -2580,8 +2740,11 @@
       <c r="C7" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -2591,8 +2754,11 @@
       <c r="C8" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -2602,8 +2768,11 @@
       <c r="C9" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -2613,8 +2782,11 @@
       <c r="C10" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -2624,8 +2796,11 @@
       <c r="C11" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -2635,8 +2810,11 @@
       <c r="C12" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2646,8 +2824,11 @@
       <c r="C13" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -2657,8 +2838,11 @@
       <c r="C14" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>15</v>
       </c>
@@ -2668,8 +2852,11 @@
       <c r="C15" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -2679,8 +2866,11 @@
       <c r="C16" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -2690,8 +2880,11 @@
       <c r="C17" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -2701,8 +2894,11 @@
       <c r="C18" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -2712,8 +2908,11 @@
       <c r="C19" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -2723,8 +2922,11 @@
       <c r="C20" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -2734,8 +2936,11 @@
       <c r="C21" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -2745,8 +2950,11 @@
       <c r="C22" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -2756,8 +2964,11 @@
       <c r="C23" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -2767,8 +2978,11 @@
       <c r="C24" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -2778,8 +2992,11 @@
       <c r="C25" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1">
         <v>384</v>
       </c>
@@ -2789,8 +3006,11 @@
       <c r="C26" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1">
         <v>442</v>
       </c>
@@ -2800,8 +3020,11 @@
       <c r="C27" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1">
         <v>23</v>
       </c>
@@ -2811,8 +3034,11 @@
       <c r="C28" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1">
         <v>24</v>
       </c>
@@ -2822,8 +3048,11 @@
       <c r="C29" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1">
         <v>25</v>
       </c>
@@ -2833,8 +3062,11 @@
       <c r="C30" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1">
         <v>26</v>
       </c>
@@ -2844,8 +3076,11 @@
       <c r="C31" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1">
         <v>27</v>
       </c>
@@ -2855,8 +3090,11 @@
       <c r="C32" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1">
         <v>28</v>
       </c>
@@ -2866,8 +3104,11 @@
       <c r="C33" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1">
         <v>29</v>
       </c>
@@ -2877,8 +3118,11 @@
       <c r="C34" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1">
         <v>543</v>
       </c>
@@ -2888,8 +3132,11 @@
       <c r="C35" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1">
         <v>30</v>
       </c>
@@ -2899,8 +3146,11 @@
       <c r="C36" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1">
         <v>31</v>
       </c>
@@ -2910,8 +3160,11 @@
       <c r="C37" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1">
         <v>32</v>
       </c>
@@ -2921,8 +3174,11 @@
       <c r="C38" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1">
         <v>33</v>
       </c>
@@ -2932,8 +3188,11 @@
       <c r="C39" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="D39" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1">
         <v>544</v>
       </c>
@@ -2943,8 +3202,11 @@
       <c r="C40" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1">
         <v>34</v>
       </c>
@@ -2954,8 +3216,11 @@
       <c r="C41" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1">
         <v>35</v>
       </c>
@@ -2965,8 +3230,11 @@
       <c r="C42" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1">
         <v>38</v>
       </c>
@@ -2976,8 +3244,11 @@
       <c r="C43" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1">
         <v>505</v>
       </c>
@@ -2987,8 +3258,11 @@
       <c r="C44" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1">
         <v>36</v>
       </c>
@@ -2998,8 +3272,11 @@
       <c r="C45" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="D45" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1">
         <v>387</v>
       </c>
@@ -3009,8 +3286,11 @@
       <c r="C46" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1">
         <v>37</v>
       </c>
@@ -3020,8 +3300,11 @@
       <c r="C47" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1">
         <v>39</v>
       </c>
@@ -3032,7 +3315,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1">
         <v>40</v>
       </c>
@@ -3043,7 +3326,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1">
         <v>41</v>
       </c>
@@ -3054,7 +3337,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1">
         <v>545</v>
       </c>
@@ -3065,7 +3348,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1">
         <v>42</v>
       </c>
@@ -3076,7 +3359,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1">
         <v>43</v>
       </c>
@@ -3087,7 +3370,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1">
         <v>44</v>
       </c>
@@ -3098,7 +3381,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1">
         <v>45</v>
       </c>
@@ -3109,7 +3392,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1">
         <v>46</v>
       </c>
@@ -3120,7 +3403,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1">
         <v>47</v>
       </c>
@@ -3131,7 +3414,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1">
         <v>48</v>
       </c>
@@ -3142,7 +3425,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1">
         <v>49</v>
       </c>
@@ -3153,7 +3436,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1">
         <v>50</v>
       </c>
@@ -3164,7 +3447,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1">
         <v>51</v>
       </c>
@@ -3175,7 +3458,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1">
         <v>52</v>
       </c>
@@ -3186,7 +3469,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1">
         <v>53</v>
       </c>
@@ -3197,7 +3480,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1">
         <v>54</v>
       </c>
@@ -3208,7 +3491,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1">
         <v>55</v>
       </c>
@@ -3219,7 +3502,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1">
         <v>57</v>
       </c>
@@ -3230,7 +3513,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1">
         <v>56</v>
       </c>
@@ -3241,7 +3524,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1">
         <v>58</v>
       </c>
@@ -3252,7 +3535,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1">
         <v>59</v>
       </c>
@@ -3263,7 +3546,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1">
         <v>60</v>
       </c>
@@ -3274,7 +3557,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1">
         <v>61</v>
       </c>
@@ -3285,7 +3568,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1">
         <v>62</v>
       </c>
@@ -3296,7 +3579,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1">
         <v>63</v>
       </c>
@@ -3307,7 +3590,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1">
         <v>64</v>
       </c>
@@ -3318,7 +3601,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1">
         <v>65</v>
       </c>
@@ -3329,7 +3612,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1">
         <v>67</v>
       </c>
@@ -3340,7 +3623,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1">
         <v>66</v>
       </c>
@@ -3351,7 +3634,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1">
         <v>68</v>
       </c>
@@ -3362,7 +3645,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1">
         <v>69</v>
       </c>
@@ -3373,7 +3656,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1">
         <v>70</v>
       </c>
@@ -3384,7 +3667,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1">
         <v>71</v>
       </c>
@@ -3395,7 +3678,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1">
         <v>72</v>
       </c>
@@ -3406,7 +3689,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1">
         <v>73</v>
       </c>
@@ -3417,7 +3700,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1">
         <v>74</v>
       </c>
@@ -3428,7 +3711,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1">
         <v>75</v>
       </c>
@@ -3439,7 +3722,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1">
         <v>76</v>
       </c>
@@ -3450,7 +3733,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1">
         <v>77</v>
       </c>
@@ -3461,7 +3744,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1">
         <v>78</v>
       </c>
@@ -3472,7 +3755,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1">
         <v>79</v>
       </c>
@@ -3483,7 +3766,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1">
         <v>80</v>
       </c>
@@ -3494,7 +3777,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1">
         <v>81</v>
       </c>
@@ -3505,7 +3788,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1">
         <v>82</v>
       </c>
@@ -3516,7 +3799,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1">
         <v>83</v>
       </c>
@@ -3527,7 +3810,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1">
         <v>84</v>
       </c>
@@ -3538,7 +3821,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1">
         <v>89</v>
       </c>
@@ -3549,7 +3832,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1">
         <v>85</v>
       </c>
@@ -3560,7 +3843,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1">
         <v>86</v>
       </c>
@@ -3571,7 +3854,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1">
         <v>546</v>
       </c>
@@ -3582,7 +3865,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1">
         <v>87</v>
       </c>
@@ -3593,7 +3876,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="1">
         <v>88</v>
       </c>
@@ -3604,7 +3887,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1">
         <v>90</v>
       </c>
@@ -3615,7 +3898,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="1">
         <v>91</v>
       </c>
@@ -3626,7 +3909,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="1">
         <v>92</v>
       </c>
@@ -3637,7 +3920,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1">
         <v>421</v>
       </c>
@@ -3648,7 +3931,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="1">
         <v>93</v>
       </c>
@@ -3659,7 +3942,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="1">
         <v>94</v>
       </c>
@@ -3670,7 +3953,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="1">
         <v>95</v>
       </c>
@@ -3681,7 +3964,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="1">
         <v>99</v>
       </c>
@@ -3692,7 +3975,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="1">
         <v>96</v>
       </c>
@@ -3703,7 +3986,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="1">
         <v>97</v>
       </c>
@@ -3714,7 +3997,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="1">
         <v>98</v>
       </c>
@@ -3725,7 +4008,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="1">
         <v>100</v>
       </c>
@@ -3736,7 +4019,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="1">
         <v>101</v>
       </c>
@@ -3747,7 +4030,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="1">
         <v>577</v>
       </c>
@@ -3758,7 +4041,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="1">
         <v>102</v>
       </c>
@@ -3769,7 +4052,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="1">
         <v>103</v>
       </c>
@@ -3780,7 +4063,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="1">
         <v>104</v>
       </c>
@@ -3791,7 +4074,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="1">
         <v>105</v>
       </c>
@@ -3802,7 +4085,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="1">
         <v>106</v>
       </c>
@@ -3813,7 +4096,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="1">
         <v>107</v>
       </c>
@@ -3824,7 +4107,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="1">
         <v>108</v>
       </c>
@@ -3835,7 +4118,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="1">
         <v>109</v>
       </c>
@@ -3846,7 +4129,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="1">
         <v>110</v>
       </c>
@@ -3857,7 +4140,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="1">
         <v>547</v>
       </c>
@@ -3868,7 +4151,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="1">
         <v>111</v>
       </c>
@@ -3879,7 +4162,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="1">
         <v>113</v>
       </c>
@@ -3890,7 +4173,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="1">
         <v>112</v>
       </c>
@@ -3901,7 +4184,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="1">
         <v>116</v>
       </c>
@@ -3912,7 +4195,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="1">
         <v>114</v>
       </c>
@@ -3923,7 +4206,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="1">
         <v>115</v>
       </c>
@@ -3934,7 +4217,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="1">
         <v>578</v>
       </c>
@@ -3945,7 +4228,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="1">
         <v>118</v>
       </c>
@@ -3956,7 +4239,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="1">
         <v>117</v>
       </c>
@@ -3967,7 +4250,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="1">
         <v>119</v>
       </c>
@@ -3978,7 +4261,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="1">
         <v>121</v>
       </c>
@@ -3989,7 +4272,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="1">
         <v>120</v>
       </c>
@@ -4000,7 +4283,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="1">
         <v>422</v>
       </c>
@@ -4011,7 +4294,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="1">
         <v>122</v>
       </c>
@@ -4022,7 +4305,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="1">
         <v>123</v>
       </c>
@@ -4033,7 +4316,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="1">
         <v>125</v>
       </c>
@@ -4044,7 +4327,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="1">
         <v>124</v>
       </c>
@@ -4055,7 +4338,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="1">
         <v>126</v>
       </c>
@@ -4066,7 +4349,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="1">
         <v>128</v>
       </c>
@@ -4077,7 +4360,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="1">
         <v>127</v>
       </c>
@@ -4088,7 +4371,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="1">
         <v>536</v>
       </c>
@@ -4099,7 +4382,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="1">
         <v>129</v>
       </c>
@@ -4110,7 +4393,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="1">
         <v>130</v>
       </c>
@@ -4121,7 +4404,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="1">
         <v>131</v>
       </c>
@@ -4132,7 +4415,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="1">
         <v>132</v>
       </c>
@@ -4143,7 +4426,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="1">
         <v>133</v>
       </c>
@@ -4154,7 +4437,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="1">
         <v>134</v>
       </c>
@@ -4165,7 +4448,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="1">
         <v>135</v>
       </c>
@@ -4176,7 +4459,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="1">
         <v>450</v>
       </c>
@@ -4187,7 +4470,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="1">
         <v>136</v>
       </c>
@@ -4198,7 +4481,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="1">
         <v>137</v>
       </c>
@@ -4209,7 +4492,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="1">
         <v>513</v>
       </c>
@@ -4220,7 +4503,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="1">
         <v>138</v>
       </c>
@@ -4231,7 +4514,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="1">
         <v>139</v>
       </c>
@@ -4242,7 +4525,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="1">
         <v>140</v>
       </c>
@@ -4253,7 +4536,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="1">
         <v>141</v>
       </c>
@@ -4264,7 +4547,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="1">
         <v>142</v>
       </c>
@@ -4275,7 +4558,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="1">
         <v>143</v>
       </c>
@@ -4286,7 +4569,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="1">
         <v>144</v>
       </c>
@@ -4297,7 +4580,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="1">
         <v>145</v>
       </c>
@@ -4308,7 +4591,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="165" spans="1:3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="1">
         <v>146</v>
       </c>
@@ -4319,7 +4602,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="1">
         <v>147</v>
       </c>
@@ -4330,7 +4613,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="1">
         <v>148</v>
       </c>
@@ -4341,7 +4624,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="168" spans="1:3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="1">
         <v>149</v>
       </c>
@@ -4352,7 +4635,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="1">
         <v>150</v>
       </c>
@@ -4363,7 +4646,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="170" spans="1:3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="1">
         <v>153</v>
       </c>
@@ -4374,7 +4657,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="1">
         <v>151</v>
       </c>
@@ -4385,7 +4668,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="1">
         <v>152</v>
       </c>
@@ -4396,7 +4679,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="1">
         <v>154</v>
       </c>
@@ -4407,7 +4690,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="174" spans="1:3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="1">
         <v>579</v>
       </c>
@@ -4418,7 +4701,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="1">
         <v>155</v>
       </c>
@@ -4429,7 +4712,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="1">
         <v>156</v>
       </c>
@@ -4440,7 +4723,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="1">
         <v>157</v>
       </c>
@@ -4451,7 +4734,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="1">
         <v>158</v>
       </c>
@@ -4462,7 +4745,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="1">
         <v>159</v>
       </c>
@@ -4473,7 +4756,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="1">
         <v>161</v>
       </c>
@@ -4484,7 +4767,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="1">
         <v>160</v>
       </c>
@@ -4495,7 +4778,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="1">
         <v>162</v>
       </c>
@@ -4506,7 +4789,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="183" spans="1:3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="1">
         <v>163</v>
       </c>
@@ -4517,7 +4800,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="184" spans="1:3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="1">
         <v>164</v>
       </c>
@@ -4528,7 +4811,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="185" spans="1:3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="1">
         <v>167</v>
       </c>
@@ -4539,7 +4822,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="1">
         <v>165</v>
       </c>
@@ -4550,7 +4833,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="1">
         <v>166</v>
       </c>
@@ -4561,7 +4844,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="1">
         <v>170</v>
       </c>
@@ -4572,7 +4855,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="189" spans="1:3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="1">
         <v>168</v>
       </c>
@@ -4583,7 +4866,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="190" spans="1:3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="1">
         <v>169</v>
       </c>
@@ -4594,7 +4877,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="191" spans="1:3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="1">
         <v>171</v>
       </c>
@@ -4605,7 +4888,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="1">
         <v>173</v>
       </c>
@@ -4616,7 +4899,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="193" spans="1:3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="1">
         <v>172</v>
       </c>
@@ -4627,7 +4910,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="1">
         <v>174</v>
       </c>
@@ -4638,7 +4921,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="1">
         <v>175</v>
       </c>
@@ -4649,7 +4932,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="196" spans="1:3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="1">
         <v>401</v>
       </c>
@@ -4660,7 +4943,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="197" spans="1:3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="1">
         <v>176</v>
       </c>
@@ -4671,7 +4954,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="198" spans="1:3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="1">
         <v>177</v>
       </c>
@@ -4682,7 +4965,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="199" spans="1:3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="1">
         <v>178</v>
       </c>
@@ -4693,7 +4976,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="200" spans="1:3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="1">
         <v>179</v>
       </c>
@@ -4704,7 +4987,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="201" spans="1:3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="1">
         <v>569</v>
       </c>
@@ -4715,7 +4998,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="202" spans="1:3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="1">
         <v>181</v>
       </c>
@@ -4726,7 +5009,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="203" spans="1:3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="1">
         <v>180</v>
       </c>
@@ -4737,7 +5020,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="204" spans="1:3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="1">
         <v>182</v>
       </c>
@@ -4748,7 +5031,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="205" spans="1:3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="1">
         <v>184</v>
       </c>
@@ -4759,7 +5042,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="206" spans="1:3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="1">
         <v>183</v>
       </c>
@@ -4770,7 +5053,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="207" spans="1:3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="1">
         <v>185</v>
       </c>
@@ -4781,7 +5064,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="208" spans="1:3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="1">
         <v>186</v>
       </c>
@@ -4792,7 +5075,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="1">
         <v>187</v>
       </c>
@@ -4803,7 +5086,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="210" spans="1:3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="1">
         <v>537</v>
       </c>
@@ -4814,7 +5097,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="211" spans="1:3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="1">
         <v>188</v>
       </c>
@@ -4825,7 +5108,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="212" spans="1:3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="1">
         <v>194</v>
       </c>
@@ -4836,7 +5119,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="213" spans="1:3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="1">
         <v>189</v>
       </c>
@@ -4847,7 +5130,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="214" spans="1:3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="1">
         <v>190</v>
       </c>
@@ -4858,7 +5141,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="215" spans="1:3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="1">
         <v>549</v>
       </c>
@@ -4869,7 +5152,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="216" spans="1:3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="1">
         <v>191</v>
       </c>
@@ -4880,7 +5163,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="217" spans="1:3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="1">
         <v>192</v>
       </c>
@@ -4891,7 +5174,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="218" spans="1:3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="1">
         <v>193</v>
       </c>
@@ -4902,7 +5185,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="219" spans="1:3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="1">
         <v>550</v>
       </c>
@@ -4913,7 +5196,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="220" spans="1:3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="1">
         <v>528</v>
       </c>
@@ -4924,7 +5207,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="221" spans="1:3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="1">
         <v>539</v>
       </c>
@@ -4935,7 +5218,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="222" spans="1:3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="1">
         <v>195</v>
       </c>
@@ -4946,7 +5229,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="223" spans="1:3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="1">
         <v>196</v>
       </c>
@@ -4957,7 +5240,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="224" spans="1:3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" s="1">
         <v>197</v>
       </c>
@@ -4968,7 +5251,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="225" spans="1:3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="1">
         <v>517</v>
       </c>
@@ -4979,7 +5262,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="226" spans="1:3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="1">
         <v>198</v>
       </c>
@@ -4990,7 +5273,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="227" spans="1:3">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" s="1">
         <v>199</v>
       </c>
@@ -5001,7 +5284,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="228" spans="1:3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="1">
         <v>571</v>
       </c>
@@ -5012,7 +5295,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="229" spans="1:3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" s="1">
         <v>201</v>
       </c>
@@ -5023,7 +5306,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="230" spans="1:3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" s="1">
         <v>200</v>
       </c>
@@ -5034,7 +5317,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="231" spans="1:3">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="1">
         <v>202</v>
       </c>
@@ -5045,7 +5328,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="232" spans="1:3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" s="1">
         <v>203</v>
       </c>
@@ -5056,7 +5339,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="233" spans="1:3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="1">
         <v>205</v>
       </c>
@@ -5067,7 +5350,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="234" spans="1:3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="1">
         <v>204</v>
       </c>
@@ -5078,7 +5361,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="235" spans="1:3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" s="1">
         <v>207</v>
       </c>
@@ -5089,7 +5372,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="236" spans="1:3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="1">
         <v>206</v>
       </c>
@@ -5100,7 +5383,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="237" spans="1:3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="1">
         <v>208</v>
       </c>
@@ -5111,7 +5394,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="238" spans="1:3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="1">
         <v>209</v>
       </c>
@@ -5122,7 +5405,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="239" spans="1:3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="1">
         <v>211</v>
       </c>
@@ -5133,7 +5416,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="240" spans="1:3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="1">
         <v>210</v>
       </c>
@@ -5144,7 +5427,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="241" spans="1:3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="1">
         <v>212</v>
       </c>
@@ -5155,7 +5438,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="242" spans="1:3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="1">
         <v>213</v>
       </c>
@@ -5166,7 +5449,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="243" spans="1:3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="1">
         <v>214</v>
       </c>
@@ -5177,7 +5460,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="244" spans="1:3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="1">
         <v>215</v>
       </c>
@@ -5188,7 +5471,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="245" spans="1:3">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="1">
         <v>216</v>
       </c>
@@ -5199,7 +5482,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="246" spans="1:3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="1">
         <v>218</v>
       </c>
@@ -5210,7 +5493,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="247" spans="1:3">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="1">
         <v>217</v>
       </c>
@@ -5221,7 +5504,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="248" spans="1:3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" s="1">
         <v>219</v>
       </c>
@@ -5232,7 +5515,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="249" spans="1:3">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" s="1">
         <v>552</v>
       </c>
@@ -5243,7 +5526,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="250" spans="1:3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" s="1">
         <v>220</v>
       </c>
@@ -5254,7 +5537,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="251" spans="1:3">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" s="1">
         <v>221</v>
       </c>
@@ -5265,7 +5548,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="252" spans="1:3">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" s="1">
         <v>222</v>
       </c>
@@ -5276,7 +5559,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="253" spans="1:3">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="1">
         <v>223</v>
       </c>
@@ -5287,7 +5570,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="254" spans="1:3">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" s="1">
         <v>224</v>
       </c>
@@ -5298,7 +5581,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="255" spans="1:3">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" s="1">
         <v>225</v>
       </c>
@@ -5309,7 +5592,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="256" spans="1:3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" s="1">
         <v>226</v>
       </c>
@@ -5320,7 +5603,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="257" spans="1:3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" s="1">
         <v>227</v>
       </c>
@@ -5331,7 +5614,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="258" spans="1:3">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" s="1">
         <v>228</v>
       </c>
@@ -5342,7 +5625,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="259" spans="1:3">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="1">
         <v>229</v>
       </c>
@@ -5353,7 +5636,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="260" spans="1:3">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" s="1">
         <v>230</v>
       </c>
@@ -5364,7 +5647,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="261" spans="1:3">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="1">
         <v>231</v>
       </c>
@@ -5375,7 +5658,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="262" spans="1:3">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A262" s="1">
         <v>232</v>
       </c>
@@ -5386,7 +5669,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="263" spans="1:3">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" s="1">
         <v>233</v>
       </c>
@@ -5397,7 +5680,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="264" spans="1:3">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" s="1">
         <v>234</v>
       </c>
@@ -5408,7 +5691,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="265" spans="1:3">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" s="1">
         <v>235</v>
       </c>
@@ -5419,7 +5702,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="266" spans="1:3">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" s="1">
         <v>236</v>
       </c>
@@ -5430,7 +5713,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="267" spans="1:3">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" s="1">
         <v>237</v>
       </c>
@@ -5441,7 +5724,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="268" spans="1:3">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" s="1">
         <v>238</v>
       </c>
@@ -5452,7 +5735,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="269" spans="1:3">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" s="1">
         <v>239</v>
       </c>
@@ -5463,7 +5746,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="270" spans="1:3">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" s="1">
         <v>241</v>
       </c>
@@ -5474,7 +5757,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="271" spans="1:3">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" s="1">
         <v>240</v>
       </c>
@@ -5485,7 +5768,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="272" spans="1:3">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" s="1">
         <v>242</v>
       </c>
@@ -5496,7 +5779,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="273" spans="1:3">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A273" s="1">
         <v>243</v>
       </c>
@@ -5507,7 +5790,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="274" spans="1:3">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" s="1">
         <v>244</v>
       </c>
@@ -5518,7 +5801,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="275" spans="1:3">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A275" s="1">
         <v>431</v>
       </c>
@@ -5529,7 +5812,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="276" spans="1:3">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" s="1">
         <v>554</v>
       </c>
@@ -5540,7 +5823,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="277" spans="1:3">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" s="1">
         <v>245</v>
       </c>
@@ -5551,7 +5834,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="278" spans="1:3">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" s="1">
         <v>246</v>
       </c>
@@ -5562,7 +5845,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="279" spans="1:3">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" s="1">
         <v>247</v>
       </c>
@@ -5573,7 +5856,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="280" spans="1:3">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" s="1">
         <v>249</v>
       </c>
@@ -5584,7 +5867,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="281" spans="1:3">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" s="1">
         <v>248</v>
       </c>
@@ -5595,7 +5878,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="282" spans="1:3">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" s="1">
         <v>555</v>
       </c>
@@ -5606,7 +5889,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="283" spans="1:3">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" s="1">
         <v>556</v>
       </c>
@@ -5617,7 +5900,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="284" spans="1:3">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" s="1">
         <v>531</v>
       </c>
@@ -5628,7 +5911,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="285" spans="1:3">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" s="1">
         <v>250</v>
       </c>
@@ -5639,7 +5922,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="286" spans="1:3">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" s="1">
         <v>251</v>
       </c>
@@ -5650,7 +5933,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="287" spans="1:3">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" s="1">
         <v>252</v>
       </c>
@@ -5661,7 +5944,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="288" spans="1:3">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" s="1">
         <v>258</v>
       </c>
@@ -5672,7 +5955,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="289" spans="1:3">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" s="1">
         <v>253</v>
       </c>
@@ -5683,7 +5966,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="290" spans="1:3">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A290" s="1">
         <v>254</v>
       </c>
@@ -5694,7 +5977,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="291" spans="1:3">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" s="1">
         <v>557</v>
       </c>
@@ -5705,7 +5988,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="292" spans="1:3">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" s="1">
         <v>255</v>
       </c>
@@ -5716,7 +5999,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="293" spans="1:3">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" s="1">
         <v>256</v>
       </c>
@@ -5727,7 +6010,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="294" spans="1:3">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" s="1">
         <v>257</v>
       </c>
@@ -5738,7 +6021,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="295" spans="1:3">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" s="1">
         <v>259</v>
       </c>
@@ -5749,7 +6032,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="296" spans="1:3">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" s="1">
         <v>260</v>
       </c>
@@ -5760,7 +6043,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="297" spans="1:3">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" s="1">
         <v>261</v>
       </c>
@@ -5771,7 +6054,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="298" spans="1:3">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" s="1">
         <v>262</v>
       </c>
@@ -5782,7 +6065,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="299" spans="1:3">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" s="1">
         <v>263</v>
       </c>
@@ -5793,7 +6076,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="300" spans="1:3">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" s="1">
         <v>264</v>
       </c>
@@ -5804,7 +6087,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="301" spans="1:3">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" s="1">
         <v>265</v>
       </c>
@@ -5815,7 +6098,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="302" spans="1:3">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" s="1">
         <v>266</v>
       </c>
@@ -5826,7 +6109,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="303" spans="1:3">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" s="1">
         <v>267</v>
       </c>
@@ -5837,7 +6120,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="304" spans="1:3">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" s="1">
         <v>271</v>
       </c>
@@ -5848,7 +6131,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="305" spans="1:3">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" s="1">
         <v>268</v>
       </c>
@@ -5859,7 +6142,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="306" spans="1:3">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" s="1">
         <v>269</v>
       </c>
@@ -5870,7 +6153,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="307" spans="1:3">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" s="1">
         <v>270</v>
       </c>
@@ -5881,7 +6164,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="308" spans="1:3">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" s="1">
         <v>281</v>
       </c>
@@ -5892,7 +6175,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="309" spans="1:3">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A309" s="1">
         <v>272</v>
       </c>
@@ -5903,7 +6186,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="310" spans="1:3">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" s="1">
         <v>432</v>
       </c>
@@ -5914,7 +6197,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="311" spans="1:3">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A311" s="1">
         <v>273</v>
       </c>
@@ -5925,7 +6208,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="312" spans="1:3">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A312" s="1">
         <v>274</v>
       </c>
@@ -5936,7 +6219,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="313" spans="1:3">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" s="1">
         <v>275</v>
       </c>
@@ -5947,7 +6230,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="314" spans="1:3">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" s="1">
         <v>276</v>
       </c>
@@ -5958,7 +6241,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="315" spans="1:3">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A315" s="1">
         <v>277</v>
       </c>
@@ -5969,7 +6252,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="316" spans="1:3">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A316" s="1">
         <v>278</v>
       </c>
@@ -5980,7 +6263,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="317" spans="1:3">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A317" s="1">
         <v>279</v>
       </c>
@@ -5991,7 +6274,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="318" spans="1:3">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A318" s="1">
         <v>280</v>
       </c>
@@ -6002,7 +6285,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="319" spans="1:3">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" s="1">
         <v>282</v>
       </c>
@@ -6013,7 +6296,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="320" spans="1:3">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" s="1">
         <v>283</v>
       </c>
@@ -6024,7 +6307,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="321" spans="1:3">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A321" s="1">
         <v>284</v>
       </c>
@@ -6035,7 +6318,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="322" spans="1:3">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A322" s="1">
         <v>285</v>
       </c>
@@ -6046,7 +6329,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="323" spans="1:3">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" s="1">
         <v>286</v>
       </c>
@@ -6057,7 +6340,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="324" spans="1:3">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" s="1">
         <v>287</v>
       </c>
@@ -6068,7 +6351,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="325" spans="1:3">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" s="1">
         <v>289</v>
       </c>
@@ -6079,7 +6362,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="326" spans="1:3">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A326" s="1">
         <v>288</v>
       </c>
@@ -6090,7 +6373,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="327" spans="1:3">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A327" s="1">
         <v>540</v>
       </c>
@@ -6101,7 +6384,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="328" spans="1:3">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" s="1">
         <v>290</v>
       </c>
@@ -6112,7 +6395,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="329" spans="1:3">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" s="1">
         <v>291</v>
       </c>
@@ -6123,7 +6406,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="330" spans="1:3">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" s="1">
         <v>292</v>
       </c>
@@ -6134,7 +6417,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="331" spans="1:3">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" s="1">
         <v>293</v>
       </c>
@@ -6145,7 +6428,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="332" spans="1:3">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" s="1">
         <v>297</v>
       </c>
@@ -6156,7 +6439,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="333" spans="1:3">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" s="1">
         <v>294</v>
       </c>
@@ -6167,7 +6450,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="334" spans="1:3">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A334" s="1">
         <v>295</v>
       </c>
@@ -6178,7 +6461,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="335" spans="1:3">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A335" s="1">
         <v>296</v>
       </c>
@@ -6189,7 +6472,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="336" spans="1:3">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" s="1">
         <v>298</v>
       </c>
@@ -6200,7 +6483,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="337" spans="1:3">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A337" s="1">
         <v>299</v>
       </c>
@@ -6211,7 +6494,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="338" spans="1:3">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A338" s="1">
         <v>301</v>
       </c>
@@ -6222,7 +6505,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="339" spans="1:3">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A339" s="1">
         <v>300</v>
       </c>
@@ -6233,7 +6516,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="340" spans="1:3">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" s="1">
         <v>302</v>
       </c>
@@ -6244,7 +6527,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="341" spans="1:3">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A341" s="1">
         <v>303</v>
       </c>
@@ -6255,7 +6538,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="342" spans="1:3">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" s="1">
         <v>304</v>
       </c>
@@ -6266,7 +6549,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="343" spans="1:3">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A343" s="1">
         <v>305</v>
       </c>
@@ -6277,7 +6560,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="344" spans="1:3">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A344" s="1">
         <v>306</v>
       </c>
@@ -6288,7 +6571,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="345" spans="1:3">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A345" s="1">
         <v>307</v>
       </c>
@@ -6299,7 +6582,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="346" spans="1:3">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A346" s="1">
         <v>308</v>
       </c>
@@ -6310,7 +6593,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="347" spans="1:3">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A347" s="1">
         <v>309</v>
       </c>
@@ -6321,7 +6604,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="348" spans="1:3">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A348" s="1">
         <v>310</v>
       </c>
@@ -6332,7 +6615,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="349" spans="1:3">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A349" s="1">
         <v>311</v>
       </c>
@@ -6343,7 +6626,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="350" spans="1:3">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A350" s="1">
         <v>312</v>
       </c>
@@ -6354,7 +6637,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="351" spans="1:3">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A351" s="1">
         <v>313</v>
       </c>
@@ -6365,7 +6648,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="352" spans="1:3">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A352" s="1">
         <v>314</v>
       </c>
@@ -6376,7 +6659,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="353" spans="1:3">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A353" s="1">
         <v>315</v>
       </c>
@@ -6387,7 +6670,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="354" spans="1:3">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A354" s="1">
         <v>316</v>
       </c>
@@ -6398,7 +6681,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="355" spans="1:3">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A355" s="1">
         <v>317</v>
       </c>

</xml_diff>